<commit_message>
Adding github account links
</commit_message>
<xml_diff>
--- a/documentation/ProposalContentStudentNameRev02.xlsx
+++ b/documentation/ProposalContentStudentNameRev02.xlsx
@@ -26,12 +26,6 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>Project website</t>
-  </si>
-  <si>
-    <t>Username.github.io/SensorEffector</t>
-  </si>
-  <si>
     <t>My project will</t>
   </si>
   <si>
@@ -72,6 +66,12 @@
   </si>
   <si>
     <t>First Last</t>
+  </si>
+  <si>
+    <t>https://github.com/publicusername/SensorEffector</t>
+  </si>
+  <si>
+    <t>Project repository</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,70 +453,70 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +554,7 @@
       </c>
       <c r="D1" s="2" t="str">
         <f>DataEntry!A4</f>
-        <v>Project website</v>
+        <v>Project repository</v>
       </c>
       <c r="E1" s="2" t="str">
         <f>DataEntry!A5</f>
@@ -616,7 +616,7 @@
       </c>
       <c r="D2" s="2" t="str">
         <f>DataEntry!B4</f>
-        <v>Username.github.io/SensorEffector</v>
+        <v>https://github.com/publicusername/SensorEffector</v>
       </c>
       <c r="E2" s="2">
         <f>DataEntry!B5</f>

</xml_diff>

<commit_message>
Improved clarity for next time
</commit_message>
<xml_diff>
--- a/documentation/ProposalContentStudentNameRev02.xlsx
+++ b/documentation/ProposalContentStudentNameRev02.xlsx
@@ -26,9 +26,6 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>My project will</t>
-  </si>
-  <si>
     <t>The database will store</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Project repository</t>
+  </si>
+  <si>
+    <t>SensorEffector choice</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,70 +453,70 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -558,7 +558,7 @@
       </c>
       <c r="E1" s="2" t="str">
         <f>DataEntry!A5</f>
-        <v>My project will</v>
+        <v>SensorEffector choice</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>DataEntry!A6</f>

</xml_diff>